<commit_message>
Project work data driven framework
</commit_message>
<xml_diff>
--- a/test_data/live_demo.xlsx
+++ b/test_data/live_demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arrowelectronics-my.sharepoint.com/personal/jui_shah_einfochips_com/Documents/Desktop/python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\framework_project\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{6125BCC9-E53F-4991-8DAD-10E362DF9526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26C13FC4-1F3D-416D-B630-2BCA67BA282D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41097045-9E04-492B-95B5-42C19202144E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2326B254-D626-4E68-9828-7823A01C564B}"/>
   </bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>